<commit_message>
add R content and images
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/coding_code_JSE/appendix materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A1EDB6-A5BE-2C44-BDDC-C390D5AD4F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80633160-1227-974A-9DF7-262B731FC227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="740" windowWidth="36920" windowHeight="18640" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="240" yWindow="720" windowWidth="36920" windowHeight="18640" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="249">
   <si>
     <t>code comment</t>
   </si>
@@ -492,9 +492,6 @@
     <t># Estimate Initial concentration of N15-NO3 relative to Ar</t>
   </si>
   <si>
-    <t>N15_NO3_O_D &lt;- 40*((carboys[carboys$CarboyID == "D",]$EstN15NO3) + (0.7*RstN/(1+RstN)))/(subset(gas, gas$carboy == "D")$Ar[1])</t>
-  </si>
-  <si>
     <t xml:space="preserve"># Estimate fraction of labeled nitrate that gets denitrified </t>
   </si>
   <si>
@@ -600,9 +597,6 @@
     <t>abline(v = upperCIBound, lty = 2, col = "blue")</t>
   </si>
   <si>
-    <t>nmle &lt;- function(P, t, y, N15_NO3_O){   yhat &lt;- N15_NO3_O * (1-exp(-P[1]*t))   -sum(dnorm(y,yhat,exp(P[2]), log = T)) }</t>
-  </si>
-  <si>
     <t>plot(x = predictionTimesD, y = predictionD, col = "blue", type = "l", xlab = "" , ylab = "", ylim = c(0,0.08), main = "Mesocosm D", las = 1)</t>
   </si>
   <si>
@@ -619,13 +613,207 @@
   </si>
   <si>
     <t>script fragments -- incorrect dimensions for variable</t>
+  </si>
+  <si>
+    <t>nmle &lt;- function(P, t, y, N15_NO3_O){   yhat &lt;- N15_NO3_O * (1 - exp(-P[1]*t)) - sum(dnorm(y, yhat, exp(P[2]), log = T)) }</t>
+  </si>
+  <si>
+    <t>N15_NO3_O_D &lt;- 40*((carboys[carboys$CarboyID == "D",]$EstN15NO3) + (0.7*RstN/(1 +RstN)))/(subset(gas, gas$carboy == "D")$Ar[1])</t>
+  </si>
+  <si>
+    <t>cleaning working environment</t>
+  </si>
+  <si>
+    <t>loading functions written in another R script</t>
+  </si>
+  <si>
+    <t>loading data, specifying full path to access data</t>
+  </si>
+  <si>
+    <t>filtering rows, using brackets, relational statement (%in%), logical (!)</t>
+  </si>
+  <si>
+    <t>create new column, mutate existing column, change data type</t>
+  </si>
+  <si>
+    <t>comment on code below</t>
+  </si>
+  <si>
+    <t>create new variable, by mutating existing column and using previously defined variable </t>
+  </si>
+  <si>
+    <t>creating new column, using previously defined variable </t>
+  </si>
+  <si>
+    <t>create new variable, by mutating existing variables</t>
+  </si>
+  <si>
+    <t>comment on units</t>
+  </si>
+  <si>
+    <t>user-defined function which takes multiple inputs, filters a vector using brackets, calculates values based on variables and function output</t>
+  </si>
+  <si>
+    <t>comment on new section of code</t>
+  </si>
+  <si>
+    <t>create new object, filter rows, using subset(), relational statement (==), select column using $</t>
+  </si>
+  <si>
+    <t>create a new object, filter rows, using subset(), relational statement (==), select column using $</t>
+  </si>
+  <si>
+    <t>create a new object, filter elements of object using brackets, relational statement (is.na) and logical (!) </t>
+  </si>
+  <si>
+    <t>create a new object, filter elements of object using brackets, relational statement (is.na) and logical (!)</t>
+  </si>
+  <si>
+    <t>comment on action taken in code below</t>
+  </si>
+  <si>
+    <t>mutate existing object, filter elements of object using brackets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filters rows (using brackets) and a relational statement (==), selects column (with $), then filters rows using subset() and a relational statement (==), selects column from filtered data and pulls out index of column with [] </t>
+  </si>
+  <si>
+    <t>comment on action of code below</t>
+  </si>
+  <si>
+    <t>create new variable, based on previously defined variable</t>
+  </si>
+  <si>
+    <t>comment on action for code below</t>
+  </si>
+  <si>
+    <t>implementing base R function, using: user-defined function (nmle), naming function arguments, imputing previously defined variables (e.g. timeE), imputing hard coded values (e.g. c(1,0.01), saving function output as new object</t>
+  </si>
+  <si>
+    <t>pulling off named function output using $, filtering elements using brackets</t>
+  </si>
+  <si>
+    <t>create new variable, mutate previously defined variable</t>
+  </si>
+  <si>
+    <t>create new variable, mutate previously defined variables</t>
+  </si>
+  <si>
+    <t>create new variable, pull off named function output using $, filter elements using brackets</t>
+  </si>
+  <si>
+    <t>starts graphics driver from macOS system</t>
+  </si>
+  <si>
+    <t>splitting the plotting window</t>
+  </si>
+  <si>
+    <t>creating new object, using values of previously defined variable, named arguments</t>
+  </si>
+  <si>
+    <t>creating new object, using values of previously defined variables</t>
+  </si>
+  <si>
+    <t>scatterplot of previously defined objects, specify color of points, type of line, axis labels, plot title, y-axis limits, orientation of axis ticks</t>
+  </si>
+  <si>
+    <t>adding points to plot, based on previously defined objects, specifying plotting character/shape</t>
+  </si>
+  <si>
+    <t>adding title to plot, using expression() for exponents and subscripts, specifies placement of title (relative to plot edge), specifying font size for subtitle</t>
+  </si>
+  <si>
+    <t>adding title to plot, specifies placement of title, specifying font size for subtitle</t>
+  </si>
+  <si>
+    <t>adds legend to plot, location of lengend, labels for legend, line types in legend, colors in legend, plotting characters in legend</t>
+  </si>
+  <si>
+    <t>create new variable, data summary (min)</t>
+  </si>
+  <si>
+    <t>create new variable, data summary (location of minimum – index)</t>
+  </si>
+  <si>
+    <t>create new variable, using existing variable</t>
+  </si>
+  <si>
+    <t>create new matrix object using previously defined variables</t>
+  </si>
+  <si>
+    <t>create a new variable by filtering existing dataframe using brackets and previously defined variable, selecting a column with [] and hardcoded number, filtering elements using [] and index (output from additional fitering)</t>
+  </si>
+  <si>
+    <t>create new vector</t>
+  </si>
+  <si>
+    <t>create new object based on existing variables</t>
+  </si>
+  <si>
+    <t>comment on what code below does</t>
+  </si>
+  <si>
+    <t>scatterplot of a locally defined variable and one previously defined variable, specify linetype, declare axis labels, change orientation of axis ticks</t>
+  </si>
+  <si>
+    <t>add vertical line to plot using previously defined variable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">creating a new dataframe, applying function over rows of existing dataframe, declare additional function arguments, name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arguments  </t>
+    </r>
+  </si>
+  <si>
+    <t>saving common functions in separate file</t>
+  </si>
+  <si>
+    <t>descriptive comments on actions being taken in different sections of code</t>
+  </si>
+  <si>
+    <t>full path to data</t>
+  </si>
+  <si>
+    <t>create function to estimate parameter</t>
+  </si>
+  <si>
+    <t>vertical line</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>applying same function across multiple rows</t>
+  </si>
+  <si>
+    <t>matrix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -651,6 +839,14 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -997,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+    <sheetView topLeftCell="B39" workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -1920,7 +2116,7 @@
         <v>77</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -2558,7 +2754,7 @@
         <v>77</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -2578,14 +2774,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="116.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.83203125" customWidth="1"/>
+    <col min="2" max="2" width="91.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2624,8 +2822,12 @@
       <c r="A2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -2638,11 +2840,19 @@
       <c r="A3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -2652,9 +2862,15 @@
       <c r="A4" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2666,10 +2882,18 @@
       <c r="A5" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2680,10 +2904,18 @@
       <c r="A6" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -2694,11 +2926,19 @@
       <c r="A7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -2708,8 +2948,12 @@
       <c r="A8" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2722,8 +2966,12 @@
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2736,9 +2984,15 @@
       <c r="A10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2750,11 +3004,19 @@
       <c r="A11" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -2764,9 +3026,15 @@
       <c r="A12" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -2778,8 +3046,12 @@
       <c r="A13" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -2792,11 +3064,19 @@
       <c r="A14" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2806,8 +3086,12 @@
       <c r="A15" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2820,8 +3104,12 @@
       <c r="A16" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2832,11 +3120,17 @@
     </row>
     <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+        <v>192</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>244</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -2848,8 +3142,12 @@
       <c r="A18" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2862,8 +3160,12 @@
       <c r="A19" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2876,11 +3178,19 @@
       <c r="A20" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -2890,11 +3200,19 @@
       <c r="A21" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -2904,11 +3222,19 @@
       <c r="A22" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -2918,11 +3244,19 @@
       <c r="A23" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -2932,8 +3266,12 @@
       <c r="A24" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="B24" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2946,11 +3284,19 @@
       <c r="A25" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="B25" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -2960,8 +3306,12 @@
       <c r="A26" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -2972,24 +3322,40 @@
     </row>
     <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -3000,11 +3366,17 @@
     </row>
     <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+        <v>152</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -3014,10 +3386,14 @@
     </row>
     <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+        <v>153</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -3028,10 +3404,14 @@
     </row>
     <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+        <v>154</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -3042,13 +3422,23 @@
     </row>
     <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -3056,11 +3446,17 @@
     </row>
     <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+        <v>156</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -3070,11 +3466,17 @@
     </row>
     <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+        <v>157</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -3084,10 +3486,14 @@
     </row>
     <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+        <v>158</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -3098,13 +3504,23 @@
     </row>
     <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+        <v>159</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -3112,10 +3528,14 @@
     </row>
     <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+        <v>160</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -3126,10 +3546,14 @@
     </row>
     <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -3140,10 +3564,14 @@
     </row>
     <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+        <v>162</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -3154,11 +3582,17 @@
     </row>
     <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -3168,11 +3602,17 @@
     </row>
     <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -3182,10 +3622,14 @@
     </row>
     <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+        <v>186</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -3196,10 +3640,14 @@
     </row>
     <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -3210,10 +3658,14 @@
     </row>
     <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+        <v>166</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -3224,10 +3676,14 @@
     </row>
     <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -3238,10 +3694,14 @@
     </row>
     <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+        <v>168</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -3252,10 +3712,14 @@
     </row>
     <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -3266,10 +3730,14 @@
     </row>
     <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3280,11 +3748,17 @@
     </row>
     <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+        <v>171</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -3294,11 +3768,17 @@
     </row>
     <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+        <v>172</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -3308,11 +3788,17 @@
     </row>
     <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+        <v>173</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -3322,11 +3808,17 @@
     </row>
     <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>248</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -3336,13 +3828,21 @@
     </row>
     <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
+        <v>188</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>247</v>
+      </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -3350,11 +3850,17 @@
     </row>
     <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -3364,11 +3870,17 @@
     </row>
     <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -3378,11 +3890,17 @@
     </row>
     <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -3392,39 +3910,69 @@
     </row>
     <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
     <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
     </row>
     <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+        <v>179</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -3434,10 +3982,14 @@
     </row>
     <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -3448,11 +4000,17 @@
     </row>
     <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -3462,11 +4020,17 @@
     </row>
     <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+        <v>182</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -3476,10 +4040,14 @@
     </row>
     <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
+        <v>183</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -3490,10 +4058,14 @@
     </row>
     <row r="64" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -3504,10 +4076,14 @@
     </row>
     <row r="65" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
+        <v>189</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -3518,11 +4094,17 @@
     </row>
     <row r="66" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+        <v>184</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -3532,9 +4114,11 @@
     </row>
     <row r="67" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B67" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>239</v>
+      </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>

</xml_diff>

<commit_message>
added R environment to lm Student A
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atheo\Documents\Current Research\Coding Code\QDA-tutorial-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80633160-1227-974A-9DF7-262B731FC227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615FC17-9E92-4586-9703-A44E3318DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="720" windowWidth="36920" windowHeight="18640" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="250">
   <si>
     <t>code comment</t>
   </si>
@@ -807,6 +807,9 @@
   </si>
   <si>
     <t>matrix</t>
+  </si>
+  <si>
+    <t>doesn't use data = argument</t>
   </si>
 </sst>
 </file>
@@ -1193,25 +1196,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="143.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="130.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="143.1875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1265,7 +1266,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1289,7 +1290,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1313,7 +1314,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1337,7 +1338,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1356,12 +1357,16 @@
       <c r="F6" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1381,7 +1386,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1401,7 +1406,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1429,7 +1434,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1449,7 +1454,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1471,7 +1476,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1490,12 +1495,16 @@
       <c r="F12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1515,7 +1524,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1535,7 +1544,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A15" s="2" t="s">
         <v>86</v>
       </c>
@@ -1563,7 +1572,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1583,7 +1592,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1603,7 +1612,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -1623,7 +1632,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1643,7 +1652,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1663,7 +1672,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1683,7 +1692,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1703,7 +1712,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1727,7 +1736,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
@@ -1751,7 +1760,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -1775,7 +1784,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -1799,7 +1808,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1828,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -1839,7 +1848,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -1859,7 +1868,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
@@ -1879,7 +1888,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1899,7 +1908,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
@@ -1919,7 +1928,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -1939,7 +1948,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -1963,7 +1972,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1981,7 +1990,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -2005,7 +2014,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -2029,7 +2038,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -2049,7 +2058,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -2069,7 +2078,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -2093,7 +2102,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -2121,7 +2130,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
@@ -2141,7 +2150,7 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
@@ -2173,7 +2182,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
@@ -2193,7 +2202,7 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -2225,7 +2234,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -2257,7 +2266,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2321,7 +2330,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2353,7 +2362,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2385,7 +2394,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2417,7 +2426,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2449,7 +2458,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2513,7 +2522,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -2545,7 +2554,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -2609,7 +2618,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
@@ -2641,7 +2650,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -2673,7 +2682,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
@@ -2705,7 +2714,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2737,7 +2746,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A62" s="2" t="s">
         <v>12</v>
       </c>
@@ -2761,7 +2770,7 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
@@ -2774,19 +2783,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+    <sheetView topLeftCell="B40" workbookViewId="0">
       <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="78.83203125" customWidth="1"/>
-    <col min="2" max="2" width="91.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.8125" customWidth="1"/>
+    <col min="2" max="2" width="91.8125" customWidth="1"/>
+    <col min="3" max="3" width="17.3125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2818,7 +2827,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A2" s="3" t="s">
         <v>127</v>
       </c>
@@ -2836,7 +2845,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="3" t="s">
         <v>128</v>
       </c>
@@ -2858,7 +2867,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A4" s="3" t="s">
         <v>129</v>
       </c>
@@ -2878,7 +2887,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A5" s="3" t="s">
         <v>130</v>
       </c>
@@ -2900,7 +2909,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A6" s="3" t="s">
         <v>131</v>
       </c>
@@ -2922,7 +2931,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A7" s="3" t="s">
         <v>132</v>
       </c>
@@ -2944,7 +2953,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A8" s="3" t="s">
         <v>133</v>
       </c>
@@ -2962,7 +2971,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
@@ -2980,7 +2989,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A10" s="3" t="s">
         <v>135</v>
       </c>
@@ -3000,7 +3009,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A11" s="3" t="s">
         <v>136</v>
       </c>
@@ -3022,7 +3031,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A12" s="3" t="s">
         <v>137</v>
       </c>
@@ -3042,7 +3051,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A13" s="3" t="s">
         <v>138</v>
       </c>
@@ -3060,7 +3069,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A14" s="3" t="s">
         <v>139</v>
       </c>
@@ -3082,7 +3091,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A15" s="3" t="s">
         <v>140</v>
       </c>
@@ -3100,7 +3109,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A16" s="3" t="s">
         <v>141</v>
       </c>
@@ -3118,7 +3127,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A17" s="3" t="s">
         <v>192</v>
       </c>
@@ -3138,7 +3147,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A18" s="3" t="s">
         <v>142</v>
       </c>
@@ -3156,7 +3165,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A19" s="3" t="s">
         <v>143</v>
       </c>
@@ -3174,7 +3183,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A20" s="3" t="s">
         <v>144</v>
       </c>
@@ -3196,7 +3205,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A21" s="3" t="s">
         <v>145</v>
       </c>
@@ -3218,7 +3227,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A22" s="3" t="s">
         <v>146</v>
       </c>
@@ -3240,7 +3249,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A23" s="3" t="s">
         <v>147</v>
       </c>
@@ -3262,7 +3271,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A24" s="3" t="s">
         <v>148</v>
       </c>
@@ -3280,7 +3289,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A25" s="3" t="s">
         <v>149</v>
       </c>
@@ -3302,7 +3311,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A26" s="3" t="s">
         <v>150</v>
       </c>
@@ -3320,7 +3329,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A27" s="3" t="s">
         <v>193</v>
       </c>
@@ -3346,7 +3355,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A28" s="3" t="s">
         <v>151</v>
       </c>
@@ -3364,7 +3373,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A29" s="3" t="s">
         <v>152</v>
       </c>
@@ -3384,7 +3393,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A30" s="3" t="s">
         <v>153</v>
       </c>
@@ -3402,7 +3411,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A31" s="3" t="s">
         <v>154</v>
       </c>
@@ -3420,7 +3429,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A32" s="3" t="s">
         <v>155</v>
       </c>
@@ -3444,7 +3453,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A33" s="3" t="s">
         <v>156</v>
       </c>
@@ -3464,7 +3473,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A34" s="3" t="s">
         <v>157</v>
       </c>
@@ -3484,7 +3493,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A35" s="3" t="s">
         <v>158</v>
       </c>
@@ -3502,7 +3511,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A36" s="3" t="s">
         <v>159</v>
       </c>
@@ -3526,7 +3535,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A37" s="3" t="s">
         <v>160</v>
       </c>
@@ -3544,7 +3553,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A38" s="3" t="s">
         <v>161</v>
       </c>
@@ -3562,7 +3571,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A39" s="3" t="s">
         <v>162</v>
       </c>
@@ -3580,7 +3589,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A40" s="3" t="s">
         <v>163</v>
       </c>
@@ -3600,7 +3609,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A41" s="3" t="s">
         <v>164</v>
       </c>
@@ -3620,7 +3629,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A42" s="3" t="s">
         <v>186</v>
       </c>
@@ -3638,7 +3647,7 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A43" s="3" t="s">
         <v>165</v>
       </c>
@@ -3656,7 +3665,7 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A44" s="3" t="s">
         <v>166</v>
       </c>
@@ -3674,7 +3683,7 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A45" s="3" t="s">
         <v>167</v>
       </c>
@@ -3692,7 +3701,7 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A46" s="3" t="s">
         <v>168</v>
       </c>
@@ -3710,7 +3719,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A47" s="3" t="s">
         <v>169</v>
       </c>
@@ -3728,7 +3737,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A48" s="3" t="s">
         <v>170</v>
       </c>
@@ -3746,7 +3755,7 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A49" s="3" t="s">
         <v>171</v>
       </c>
@@ -3766,7 +3775,7 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A50" s="3" t="s">
         <v>172</v>
       </c>
@@ -3786,7 +3795,7 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A51" s="3" t="s">
         <v>173</v>
       </c>
@@ -3806,7 +3815,7 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A52" s="3" t="s">
         <v>187</v>
       </c>
@@ -3826,7 +3835,7 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A53" s="3" t="s">
         <v>188</v>
       </c>
@@ -3848,7 +3857,7 @@
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A54" s="3" t="s">
         <v>174</v>
       </c>
@@ -3868,7 +3877,7 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A55" s="3" t="s">
         <v>175</v>
       </c>
@@ -3888,7 +3897,7 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A56" s="3" t="s">
         <v>176</v>
       </c>
@@ -3908,7 +3917,7 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A57" s="3" t="s">
         <v>177</v>
       </c>
@@ -3934,7 +3943,7 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A58" s="3" t="s">
         <v>178</v>
       </c>
@@ -3960,7 +3969,7 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A59" s="3" t="s">
         <v>179</v>
       </c>
@@ -3980,7 +3989,7 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A60" s="3" t="s">
         <v>180</v>
       </c>
@@ -3998,7 +4007,7 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A61" s="3" t="s">
         <v>181</v>
       </c>
@@ -4018,7 +4027,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A62" s="3" t="s">
         <v>182</v>
       </c>
@@ -4038,7 +4047,7 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A63" s="3" t="s">
         <v>183</v>
       </c>
@@ -4056,7 +4065,7 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A64" s="3" t="s">
         <v>161</v>
       </c>
@@ -4074,7 +4083,7 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A65" s="3" t="s">
         <v>189</v>
       </c>
@@ -4092,7 +4101,7 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A66" s="3" t="s">
         <v>184</v>
       </c>
@@ -4112,7 +4121,7 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="21" x14ac:dyDescent="0.65">
       <c r="A67" s="3" t="s">
         <v>185</v>
       </c>

</xml_diff>

<commit_message>
add efficiency to sourcing functions
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atheo\Documents\Current Research\Coding Code\QDA-tutorial-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615FC17-9E92-4586-9703-A44E3318DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644BA0FB-D4FC-4A2E-ADEC-287E131A3314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="251">
   <si>
     <t>code comment</t>
   </si>
@@ -810,6 +810,9 @@
   </si>
   <si>
     <t>doesn't use data = argument</t>
+  </si>
+  <si>
+    <t>reusing code instead of rewriting it</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2783,8 +2786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2862,8 +2865,12 @@
       <c r="F3" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>

</xml_diff>

<commit_message>
notes for every theme for Student A
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atheo\Documents\Current Research\Coding Code\QDA-tutorial-website\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644BA0FB-D4FC-4A2E-ADEC-287E131A3314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306DF4FD-0A5C-4A4B-8D98-AF289BEB41BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="1600" yWindow="660" windowWidth="34380" windowHeight="18500" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="255">
   <si>
     <t>code comment</t>
   </si>
@@ -276,9 +276,6 @@
     <t>note2</t>
   </si>
   <si>
-    <t>dataframe is attached, no $ are necessary</t>
-  </si>
-  <si>
     <t>R environment</t>
   </si>
   <si>
@@ -363,15 +360,9 @@
     <t>data wrangling</t>
   </si>
   <si>
-    <t>lack of reproducibility</t>
-  </si>
-  <si>
     <t>data model</t>
   </si>
   <si>
-    <t>linear regression</t>
-  </si>
-  <si>
     <t>selecting columns using $</t>
   </si>
   <si>
@@ -408,9 +399,6 @@
     <t>specify position for legend, declare text to display, colors to display with text, types of lines to display, thickness of lines displayed</t>
   </si>
   <si>
-    <t>filtering rows with relational operator (==)</t>
-  </si>
-  <si>
     <t>vector, [] used to extract elements</t>
   </si>
   <si>
@@ -525,9 +513,6 @@
     <t>quartz(width = 4.5, height = 4)</t>
   </si>
   <si>
-    <t>par(mar = c(3.5,4,3,1))</t>
-  </si>
-  <si>
     <t>predictionTimesD &lt;- seq(0,max(timeD), length.out = 100)</t>
   </si>
   <si>
@@ -607,9 +592,6 @@
   </si>
   <si>
     <t>plot(x = seq(kTotMin,kTotMax, length.out = numRows), y = -likelihoods, type = "l", xlab = "ktot (per day)", ylab = "log(Likelihood)", las = 1)</t>
-  </si>
-  <si>
-    <t>script fragments -- variable doesn't exist</t>
   </si>
   <si>
     <t>script fragments -- incorrect dimensions for variable</t>
@@ -813,6 +795,36 @@
   </si>
   <si>
     <t>reusing code instead of rewriting it</t>
+  </si>
+  <si>
+    <t>pull out MLE estimate</t>
+  </si>
+  <si>
+    <t>obtain predictions</t>
+  </si>
+  <si>
+    <t>par(mar = c(3.5, 4, 3, 1))</t>
+  </si>
+  <si>
+    <t>selecting columns using $, filtering rows with relational operator (==)</t>
+  </si>
+  <si>
+    <t>calculating the mean</t>
+  </si>
+  <si>
+    <t>reproducibility</t>
+  </si>
+  <si>
+    <t>readability</t>
+  </si>
+  <si>
+    <t>lm()</t>
+  </si>
+  <si>
+    <t>use of c() for legend text and colors</t>
+  </si>
+  <si>
+    <t>references a non-existant variable (mean instead of meanL)</t>
   </si>
 </sst>
 </file>
@@ -1197,25 +1209,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="143.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="130.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.83203125" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1226,7 +1240,7 @@
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>75</v>
@@ -1238,16 +1252,18 @@
         <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>122</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1255,21 +1271,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>77</v>
+        <v>251</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1277,23 +1293,19 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1301,23 +1313,19 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1325,23 +1333,19 @@
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1349,27 +1353,27 @@
         <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>110</v>
+        <v>252</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1377,10 +1381,10 @@
         <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1389,7 +1393,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1397,10 +1401,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1409,7 +1413,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1417,27 +1421,23 @@
         <v>72</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1445,10 +1445,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1457,7 +1457,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1465,21 +1465,21 @@
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>77</v>
+        <v>251</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1487,27 +1487,27 @@
         <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>110</v>
+        <v>252</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1515,10 +1515,10 @@
         <v>69</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1527,7 +1527,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1535,10 +1535,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1547,35 +1547,31 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1583,10 +1579,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1595,7 +1591,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1603,10 +1599,10 @@
         <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1615,7 +1611,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -1623,10 +1619,10 @@
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1635,7 +1631,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1643,10 +1639,10 @@
         <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1655,18 +1651,18 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1675,7 +1671,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1683,10 +1679,10 @@
         <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1695,7 +1691,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1703,10 +1699,10 @@
         <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1715,7 +1711,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1726,7 +1722,7 @@
         <v>107</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1734,12 +1730,12 @@
         <v>77</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +1746,7 @@
         <v>107</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1758,12 +1754,12 @@
         <v>77</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -1774,7 +1770,7 @@
         <v>107</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1782,12 +1778,12 @@
         <v>77</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -1795,10 +1791,10 @@
         <v>39</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1806,12 +1802,12 @@
         <v>77</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1815,7 @@
         <v>40</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>40</v>
@@ -1831,7 +1827,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -1842,7 +1838,7 @@
         <v>107</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1851,7 +1847,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -1862,7 +1858,7 @@
         <v>107</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1871,18 +1867,18 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1891,18 +1887,18 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1911,18 +1907,18 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1931,18 +1927,18 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1951,39 +1947,39 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>101</v>
+        <v>253</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1993,7 +1989,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -2001,23 +1997,23 @@
         <v>48</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -2025,7 +2021,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>40</v>
@@ -2034,14 +2030,14 @@
         <v>77</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -2052,7 +2048,7 @@
         <v>107</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2061,7 +2057,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -2072,7 +2068,7 @@
         <v>107</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -2081,70 +2077,70 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>77</v>
+        <v>250</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>190</v>
+        <v>254</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -2153,50 +2149,50 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2205,551 +2201,551 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>123</v>
+        <v>249</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>12</v>
       </c>
@@ -2757,23 +2753,23 @@
         <v>67</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>77</v>
+        <v>250</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
@@ -2786,19 +2782,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="78.8125" customWidth="1"/>
-    <col min="2" max="2" width="91.8125" customWidth="1"/>
-    <col min="3" max="3" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.83203125" customWidth="1"/>
+    <col min="2" max="2" width="91.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2809,7 +2805,7 @@
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>75</v>
@@ -2821,24 +2817,24 @@
         <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -2848,44 +2844,44 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2894,21 +2890,21 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2916,21 +2912,21 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2938,37 +2934,37 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2978,15 +2974,15 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2996,18 +2992,18 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -3016,40 +3012,40 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3058,15 +3054,15 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -3076,37 +3072,37 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3116,15 +3112,15 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3134,18 +3130,18 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -3154,15 +3150,15 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3172,15 +3168,15 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3190,103 +3186,103 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -3296,37 +3292,37 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -3336,41 +3332,41 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -3380,18 +3376,18 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -3400,15 +3396,15 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -3418,15 +3414,15 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -3436,42 +3432,46 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -3480,18 +3480,18 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -3500,15 +3500,15 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -3518,39 +3518,41 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -3560,15 +3562,15 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -3578,15 +3580,15 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -3596,18 +3598,18 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -3616,35 +3618,39 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>246</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -3654,15 +3660,15 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -3672,15 +3678,15 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -3690,15 +3696,15 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -3708,15 +3714,15 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -3726,15 +3732,15 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -3744,15 +3750,15 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -3762,18 +3768,18 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -3782,18 +3788,18 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -3802,18 +3808,18 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -3822,189 +3828,205 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E52" s="3"/>
+        <v>242</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G53" s="3"/>
+        <v>241</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C56" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H57" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I57" s="3"/>
+      <c r="I57" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H58" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G58" s="3" t="s">
+      <c r="I58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.65">
-      <c r="A59" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E59" s="3"/>
+      <c r="E59" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -4014,55 +4036,59 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -4072,15 +4098,15 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="64" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -4090,15 +4116,15 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="65" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -4108,18 +4134,18 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="66" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -4128,12 +4154,12 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="67" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>

</xml_diff>

<commit_message>
added notes to Student B
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306DF4FD-0A5C-4A4B-8D98-AF289BEB41BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467DD628-F76C-DE4C-9279-B3E2C6655160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="660" windowWidth="34380" windowHeight="18500" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="1600" yWindow="660" windowWidth="34380" windowHeight="18500" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="278">
   <si>
     <t>code comment</t>
   </si>
@@ -770,24 +770,15 @@
     <t>saving common functions in separate file</t>
   </si>
   <si>
-    <t>descriptive comments on actions being taken in different sections of code</t>
-  </si>
-  <si>
     <t>full path to data</t>
   </si>
   <si>
     <t>create function to estimate parameter</t>
   </si>
   <si>
-    <t>vertical line</t>
-  </si>
-  <si>
     <t>efficiency</t>
   </si>
   <si>
-    <t>applying same function across multiple rows</t>
-  </si>
-  <si>
     <t>matrix</t>
   </si>
   <si>
@@ -825,6 +816,84 @@
   </si>
   <si>
     <t>references a non-existant variable (mean instead of meanL)</t>
+  </si>
+  <si>
+    <t>filtering observations based on inclusion operator (%in%) and logical comparison (!)</t>
+  </si>
+  <si>
+    <t>mutate variable</t>
+  </si>
+  <si>
+    <t>select variable</t>
+  </si>
+  <si>
+    <t>variable selection</t>
+  </si>
+  <si>
+    <t>descriptive comment on actions taken in code below</t>
+  </si>
+  <si>
+    <t>code comment on units of calculation above</t>
+  </si>
+  <si>
+    <t>code comment marking new section of code</t>
+  </si>
+  <si>
+    <t>select variable, filter rows</t>
+  </si>
+  <si>
+    <t>filtering observations based on logical comparison</t>
+  </si>
+  <si>
+    <t>descriptive comment on action taken in code below</t>
+  </si>
+  <si>
+    <t>code comment on units of calculation below</t>
+  </si>
+  <si>
+    <t>descriptive comment on process in code below</t>
+  </si>
+  <si>
+    <t>descriptive comment on process taken in code below</t>
+  </si>
+  <si>
+    <t>filter observations</t>
+  </si>
+  <si>
+    <t>obtain point estimate</t>
+  </si>
+  <si>
+    <t>applying function across columns of matrix</t>
+  </si>
+  <si>
+    <t>repeated operations on multiple rows</t>
+  </si>
+  <si>
+    <t>obtaining likelihood estimates</t>
+  </si>
+  <si>
+    <t>obtaining minimum of likelihood estimates</t>
+  </si>
+  <si>
+    <t>locating which index corresponds to minimum</t>
+  </si>
+  <si>
+    <t>filtering observations based on index</t>
+  </si>
+  <si>
+    <t>obtaining confidence interval</t>
+  </si>
+  <si>
+    <t>obtaining lowerbound for confidence interval</t>
+  </si>
+  <si>
+    <t>obtaining upperbound for confidence interval</t>
+  </si>
+  <si>
+    <t>adjusting confidence interval lowerbound</t>
+  </si>
+  <si>
+    <t>adjusting confidence interval upperbound</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -1275,7 +1344,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>98</v>
@@ -1356,7 +1425,7 @@
         <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>106</v>
@@ -1368,7 +1437,7 @@
         <v>79</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1469,7 +1538,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>98</v>
@@ -1490,7 +1559,7 @@
         <v>107</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>106</v>
@@ -1502,7 +1571,7 @@
         <v>79</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1964,7 +2033,7 @@
         <v>99</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -2121,10 +2190,10 @@
         <v>108</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -2160,13 +2229,13 @@
         <v>106</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>99</v>
@@ -2212,13 +2281,13 @@
         <v>106</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>99</v>
@@ -2244,13 +2313,13 @@
         <v>106</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>99</v>
@@ -2276,13 +2345,13 @@
         <v>106</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>99</v>
@@ -2308,13 +2377,13 @@
         <v>106</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>99</v>
@@ -2340,13 +2409,13 @@
         <v>106</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>99</v>
@@ -2372,13 +2441,13 @@
         <v>106</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>99</v>
@@ -2404,13 +2473,13 @@
         <v>106</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>99</v>
@@ -2436,13 +2505,13 @@
         <v>106</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>99</v>
@@ -2468,13 +2537,13 @@
         <v>106</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>99</v>
@@ -2500,13 +2569,13 @@
         <v>106</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>99</v>
@@ -2532,13 +2601,13 @@
         <v>106</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>99</v>
@@ -2564,13 +2633,13 @@
         <v>106</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>99</v>
@@ -2596,13 +2665,13 @@
         <v>106</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>99</v>
@@ -2628,13 +2697,13 @@
         <v>106</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>99</v>
@@ -2660,13 +2729,13 @@
         <v>106</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>99</v>
@@ -2692,13 +2761,13 @@
         <v>106</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>99</v>
@@ -2724,13 +2793,13 @@
         <v>106</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>99</v>
@@ -2759,7 +2828,7 @@
         <v>105</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>185</v>
@@ -2782,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2791,7 +2860,7 @@
     <col min="1" max="1" width="78.83203125" customWidth="1"/>
     <col min="2" max="2" width="91.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2862,10 +2931,10 @@
         <v>235</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -2881,10 +2950,10 @@
         <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -2901,7 +2970,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>97</v>
@@ -2923,7 +2992,7 @@
         <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>97</v>
@@ -2944,7 +3013,9 @@
       <c r="C7" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>99</v>
       </c>
@@ -2966,7 +3037,9 @@
       <c r="C8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -2984,7 +3057,9 @@
       <c r="C9" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -3022,15 +3097,21 @@
       <c r="C11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>254</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
@@ -3047,8 +3128,12 @@
       <c r="D12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -3064,7 +3149,9 @@
       <c r="C13" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -3082,7 +3169,9 @@
       <c r="C14" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>99</v>
       </c>
@@ -3104,7 +3193,9 @@
       <c r="C15" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>257</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -3122,7 +3213,9 @@
       <c r="C16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3141,10 +3234,14 @@
         <v>107</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+        <v>237</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -3160,7 +3257,9 @@
       <c r="C18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>258</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -3178,7 +3277,9 @@
       <c r="C19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -3196,7 +3297,9 @@
       <c r="C20" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="E20" s="3" t="s">
         <v>99</v>
       </c>
@@ -3218,7 +3321,9 @@
       <c r="C21" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="E21" s="3" t="s">
         <v>99</v>
       </c>
@@ -3240,7 +3345,9 @@
       <c r="C22" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>260</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>99</v>
       </c>
@@ -3262,7 +3369,9 @@
       <c r="C23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>260</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>99</v>
       </c>
@@ -3284,7 +3393,9 @@
       <c r="C24" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -3302,7 +3413,9 @@
       <c r="C25" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>265</v>
+      </c>
       <c r="E25" s="3" t="s">
         <v>99</v>
       </c>
@@ -3324,7 +3437,9 @@
       <c r="C26" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -3342,7 +3457,9 @@
       <c r="C27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>99</v>
       </c>
@@ -3368,7 +3485,9 @@
       <c r="C28" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -3406,7 +3525,9 @@
       <c r="C30" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -3455,7 +3576,7 @@
         <v>107</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -3510,7 +3631,9 @@
       <c r="C35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -3540,7 +3663,9 @@
       <c r="G36" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
@@ -3554,7 +3679,9 @@
       <c r="C37" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -3582,7 +3709,7 @@
     </row>
     <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>216</v>
@@ -3635,7 +3762,7 @@
         <v>107</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3725,8 +3852,12 @@
         <v>80</v>
       </c>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3742,7 +3873,9 @@
       <c r="C47" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3760,7 +3893,9 @@
       <c r="C48" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3839,7 +3974,7 @@
         <v>99</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>107</v>
@@ -3860,17 +3995,21 @@
       <c r="C53" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="E53" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H53" s="3"/>
+      <c r="H53" s="3" t="s">
+        <v>269</v>
+      </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
@@ -3890,7 +4029,9 @@
       <c r="E54" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>270</v>
+      </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -3912,7 +4053,9 @@
       <c r="E55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>271</v>
+      </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -3950,12 +4093,14 @@
       <c r="C57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="E57" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>99</v>
@@ -3966,7 +4111,9 @@
       <c r="I57" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J57" s="3"/>
+      <c r="J57" s="3" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
@@ -3978,12 +4125,14 @@
       <c r="C58" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="E58" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>99</v>
@@ -3994,7 +4143,9 @@
       <c r="I58" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J58" s="3"/>
+      <c r="J58" s="3" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -4012,11 +4163,12 @@
       <c r="E59" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F59" s="3"/>
+      <c r="F59" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
     </row>
     <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -4028,7 +4180,9 @@
       <c r="C60" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -4052,7 +4206,9 @@
       <c r="E61" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F61" s="3"/>
+      <c r="F61" s="3" t="s">
+        <v>276</v>
+      </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -4074,7 +4230,9 @@
       <c r="E62" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>277</v>
+      </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -4090,7 +4248,9 @@
       <c r="C63" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -4127,8 +4287,12 @@
         <v>80</v>
       </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -4144,9 +4308,7 @@
       <c r="C66" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>239</v>
-      </c>
+      <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -4161,7 +4323,9 @@
       <c r="B67" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>

</xml_diff>

<commit_message>
finish digging deeper section, build site
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467DD628-F76C-DE4C-9279-B3E2C6655160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEBADB-8ACA-9A4F-95D3-344A44FC4324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="660" windowWidth="34380" windowHeight="18500" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="-36720" yWindow="1140" windowWidth="34380" windowHeight="18500" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2851,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added descriptions of code comments from student A
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEBADB-8ACA-9A4F-95D3-344A44FC4324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D308A0CA-6022-DF43-AE12-904B826E906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36720" yWindow="1140" windowWidth="34380" windowHeight="18500" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="-36720" yWindow="1140" windowWidth="34380" windowHeight="18500" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="281">
   <si>
     <t>code comment</t>
   </si>
@@ -894,6 +894,15 @@
   </si>
   <si>
     <t>adjusting confidence interval upperbound</t>
+  </si>
+  <si>
+    <t>comment on actions taken in code below</t>
+  </si>
+  <si>
+    <t>code comment on change in model</t>
+  </si>
+  <si>
+    <t>code comment on where code came from</t>
   </si>
 </sst>
 </file>
@@ -1280,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1351,9 @@
       <c r="C2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>278</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>248</v>
       </c>
@@ -1536,7 +1547,9 @@
       <c r="C11" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>279</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>248</v>
       </c>
@@ -2050,7 +2063,9 @@
       <c r="C35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>280</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -2851,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add R envir to Student B subset code
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D308A0CA-6022-DF43-AE12-904B826E906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D61FF-D3BF-CE4F-8F83-0F44D384A93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36720" yWindow="1140" windowWidth="34380" windowHeight="18500" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="282">
   <si>
     <t>code comment</t>
   </si>
@@ -903,6 +903,9 @@
   </si>
   <si>
     <t>code comment on where code came from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carboy variable can called on without referencing gas dataframe  </t>
   </si>
 </sst>
 </file>
@@ -2867,7 +2870,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3321,8 +3324,12 @@
       <c r="F20" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>281</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
@@ -3345,8 +3352,12 @@
       <c r="F21" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>281</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
@@ -3487,8 +3498,12 @@
       <c r="H27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">

</xml_diff>

<commit_message>
changes to student A code
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atheobol/Documents/Current Research/Coding Code/QDA-tutorial-website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D61FF-D3BF-CE4F-8F83-0F44D384A93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3DE66A-2448-644F-B69B-06B19614B4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36720" yWindow="1140" windowWidth="34380" windowHeight="18500" activeTab="1" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{2D21E880-D3DE-8743-96E7-71BD6CC98532}"/>
   </bookViews>
   <sheets>
     <sheet name="studentA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="284">
   <si>
     <t>code comment</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>abline(expAnterior)</t>
-  </si>
-  <si>
-    <t>summary(expAnterior)</t>
   </si>
   <si>
     <t>early &lt;- subset(RPMA2Growth, StockYear &lt; 2006)</t>
@@ -906,6 +903,15 @@
   </si>
   <si>
     <t xml:space="preserve">carboy variable can called on without referencing gas dataframe  </t>
+  </si>
+  <si>
+    <t>plot(expAnterior)</t>
+  </si>
+  <si>
+    <t>visualizes model diagnostics for linear model</t>
+  </si>
+  <si>
+    <t>diagnostic plots</t>
   </si>
 </sst>
 </file>
@@ -1292,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543E5B30-24D5-F643-81AE-246802AE36AA}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,51 +1324,47 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1370,16 +1372,16 @@
     </row>
     <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
@@ -1390,16 +1392,16 @@
     </row>
     <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
@@ -1410,19 +1412,23 @@
     </row>
     <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1433,25 +1439,25 @@
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1461,13 +1467,13 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1484,10 +1490,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1501,19 +1507,19 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1525,13 +1531,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1548,16 +1554,16 @@
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1569,25 +1575,25 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1597,13 +1603,13 @@
         <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1620,10 +1626,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1634,22 +1640,22 @@
     </row>
     <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1661,13 +1667,13 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1678,18 +1684,20 @@
     </row>
     <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>281</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>282</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>283</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1698,16 +1706,16 @@
     </row>
     <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1718,16 +1726,16 @@
     </row>
     <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1738,16 +1746,16 @@
     </row>
     <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1758,16 +1766,16 @@
     </row>
     <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1778,16 +1786,16 @@
     </row>
     <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1801,21 +1809,21 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -1825,21 +1833,21 @@
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1849,21 +1857,21 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -1873,21 +1881,21 @@
         <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -1897,13 +1905,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1914,16 +1922,16 @@
     </row>
     <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1934,16 +1942,16 @@
     </row>
     <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1954,16 +1962,16 @@
     </row>
     <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1974,16 +1982,16 @@
     </row>
     <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1994,16 +2002,16 @@
     </row>
     <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -2014,16 +2022,16 @@
     </row>
     <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2034,22 +2042,22 @@
     </row>
     <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -2061,13 +2069,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -2081,19 +2089,19 @@
         <v>5</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2105,19 +2113,19 @@
         <v>6</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2126,16 +2134,16 @@
     </row>
     <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2146,16 +2154,16 @@
     </row>
     <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -2169,19 +2177,19 @@
         <v>8</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -2193,25 +2201,25 @@
         <v>9</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -2221,13 +2229,13 @@
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -2238,34 +2246,34 @@
     </row>
     <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G43" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2273,13 +2281,13 @@
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2290,546 +2298,546 @@
     </row>
     <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G46" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G48" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G49" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G51" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G54" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G55" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G56" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G57" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G58" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G59" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G60" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G61" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -2837,19 +2845,19 @@
         <v>12</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -2869,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B82023-1D32-3F4B-85FA-FA399564971D}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2889,39 +2897,39 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -2933,42 +2941,42 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
@@ -2979,19 +2987,19 @@
     </row>
     <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -3001,19 +3009,19 @@
     </row>
     <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -3023,22 +3031,22 @@
     </row>
     <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -3047,16 +3055,16 @@
     </row>
     <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -3067,16 +3075,16 @@
     </row>
     <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -3087,16 +3095,16 @@
     </row>
     <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -3107,50 +3115,50 @@
     </row>
     <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -3159,16 +3167,16 @@
     </row>
     <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -3179,22 +3187,22 @@
     </row>
     <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -3203,16 +3211,16 @@
     </row>
     <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -3223,16 +3231,16 @@
     </row>
     <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -3243,22 +3251,22 @@
     </row>
     <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -3267,16 +3275,16 @@
     </row>
     <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -3287,16 +3295,16 @@
     </row>
     <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -3307,78 +3315,78 @@
     </row>
     <row r="20" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3387,22 +3395,22 @@
     </row>
     <row r="23" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -3411,16 +3419,16 @@
     </row>
     <row r="24" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3431,22 +3439,22 @@
     </row>
     <row r="25" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3455,16 +3463,16 @@
     </row>
     <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -3475,48 +3483,48 @@
     </row>
     <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="I27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -3527,16 +3535,16 @@
     </row>
     <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -3547,16 +3555,16 @@
     </row>
     <row r="30" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -3567,13 +3575,13 @@
     </row>
     <row r="31" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -3585,44 +3593,44 @@
     </row>
     <row r="32" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="G32" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -3633,16 +3641,16 @@
     </row>
     <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -3653,16 +3661,16 @@
     </row>
     <row r="35" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -3673,44 +3681,44 @@
     </row>
     <row r="36" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="G36" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -3721,13 +3729,13 @@
     </row>
     <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -3739,13 +3747,13 @@
     </row>
     <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -3757,16 +3765,16 @@
     </row>
     <row r="40" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -3777,22 +3785,22 @@
     </row>
     <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E41" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3801,13 +3809,13 @@
     </row>
     <row r="42" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -3819,13 +3827,13 @@
     </row>
     <row r="43" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -3837,13 +3845,13 @@
     </row>
     <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -3855,13 +3863,13 @@
     </row>
     <row r="45" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -3873,20 +3881,20 @@
     </row>
     <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -3895,16 +3903,16 @@
     </row>
     <row r="47" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -3915,16 +3923,16 @@
     </row>
     <row r="48" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3935,16 +3943,16 @@
     </row>
     <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -3955,16 +3963,16 @@
     </row>
     <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -3975,16 +3983,16 @@
     </row>
     <row r="51" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -3995,19 +4003,19 @@
     </row>
     <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -4017,50 +4025,50 @@
     </row>
     <row r="53" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="F53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
     <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E54" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -4069,22 +4077,22 @@
     </row>
     <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E55" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -4093,19 +4101,19 @@
     </row>
     <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C56" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E56" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -4115,86 +4123,86 @@
     </row>
     <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="J57" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I58" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="J58" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E59" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -4202,16 +4210,16 @@
     </row>
     <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -4222,22 +4230,22 @@
     </row>
     <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E61" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -4246,22 +4254,22 @@
     </row>
     <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="E62" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -4270,16 +4278,16 @@
     </row>
     <row r="63" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -4290,13 +4298,13 @@
     </row>
     <row r="64" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -4308,20 +4316,20 @@
     </row>
     <row r="65" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -4330,13 +4338,13 @@
     </row>
     <row r="66" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -4348,13 +4356,13 @@
     </row>
     <row r="67" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>

</xml_diff>